<commit_message>
Document: add API newest comment to home & add table review_comment
</commit_message>
<xml_diff>
--- a/Document/ReviewDalatDesign.xlsx
+++ b/Document/ReviewDalatDesign.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Giới thiệu" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="113">
   <si>
     <t>Tên project: Review Đà lạt</t>
   </si>
@@ -966,6 +966,730 @@
       </rPr>
       <t>,</t>
     </r>
+  </si>
+  <si>
+    <t>3. Bình luận review</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>review_object_id</t>
+  </si>
+  <si>
+    <t>point</t>
+  </si>
+  <si>
+    <t>review_comment_parent</t>
+  </si>
+  <si>
+    <t>context</t>
+  </si>
+  <si>
+    <t>like</t>
+  </si>
+  <si>
+    <t>dislike</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>'Người Bí Ẩn'</t>
+  </si>
+  <si>
+    <t>ON UPDATE CURRENT TIMESTAMP</t>
+  </si>
+  <si>
+    <t>'2020-01-01 00:00:00'</t>
+  </si>
+  <si>
+    <t>3. API lấy comment mới nhất hiển thị ra trang chủ</t>
+  </si>
+  <si>
+    <t>/comments/newest</t>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"author"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Ông Lão Đánh Cá"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"review_object_id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"2"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"review_object_name"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Thiền viện Trúc lâm"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"last_time"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"6 days 16 hours"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"point"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"4"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"context"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Tuyệt vời ông mặt trời\t"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"author"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Cá Vàng"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"review_object_id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"4"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"review_object_name"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Nhà Thờ"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"last_time"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"11 days 16 hours"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"point"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"5"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"author"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Người Bí Ẩn"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"review_object_id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"review_object_name"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Quảng Trường"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"last_time"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"379 days 16 hours"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"point"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"3"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"context"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Cái này hay lắm á\r\nVừa đẹp vừa xịn"</t>
+    </r>
+  </si>
+  <si>
+    <t>review_comment</t>
   </si>
 </sst>
 </file>
@@ -1019,11 +1743,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1368,10 +2093,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C76"/>
+  <dimension ref="B2:C108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="J85" sqref="J85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1696,63 +2421,222 @@
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C65" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C66" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C67" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C68" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C69" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C70" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C71" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C72" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C73" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C74" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C75" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C76" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>75</v>
+      </c>
+      <c r="C80" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>30</v>
+      </c>
+      <c r="C81" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>32</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C84" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C85" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C86" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C87" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C88" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C89" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C90" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C91" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C92" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C93" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C94" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C95" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C96" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C97" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C98" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C99" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C100" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C101" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C102" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C103" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C104" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C105" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C106" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C107" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C108" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1764,10 +2648,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I33"/>
+  <dimension ref="B2:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1971,6 +2855,9 @@
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1</v>
+      </c>
       <c r="C19" t="s">
         <v>11</v>
       </c>
@@ -1991,6 +2878,9 @@
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>2</v>
+      </c>
       <c r="C20" t="s">
         <v>43</v>
       </c>
@@ -2005,6 +2895,9 @@
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>3</v>
+      </c>
       <c r="C21" t="s">
         <v>57</v>
       </c>
@@ -2016,6 +2909,9 @@
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>4</v>
+      </c>
       <c r="C22" t="s">
         <v>60</v>
       </c>
@@ -2027,6 +2923,9 @@
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>5</v>
+      </c>
       <c r="C23" t="s">
         <v>44</v>
       </c>
@@ -2038,6 +2937,9 @@
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>6</v>
+      </c>
       <c r="C24" t="s">
         <v>45</v>
       </c>
@@ -2049,6 +2951,9 @@
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>7</v>
+      </c>
       <c r="C25" t="s">
         <v>46</v>
       </c>
@@ -2060,6 +2965,9 @@
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>8</v>
+      </c>
       <c r="C26" t="s">
         <v>47</v>
       </c>
@@ -2071,6 +2979,9 @@
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>9</v>
+      </c>
       <c r="C27" t="s">
         <v>48</v>
       </c>
@@ -2082,6 +2993,9 @@
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>10</v>
+      </c>
       <c r="C28" t="s">
         <v>49</v>
       </c>
@@ -2093,6 +3007,9 @@
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>11</v>
+      </c>
       <c r="C29" t="s">
         <v>50</v>
       </c>
@@ -2104,6 +3021,9 @@
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>12</v>
+      </c>
       <c r="C30" t="s">
         <v>51</v>
       </c>
@@ -2118,6 +3038,9 @@
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>13</v>
+      </c>
       <c r="C31" t="s">
         <v>52</v>
       </c>
@@ -2132,6 +3055,9 @@
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>14</v>
+      </c>
       <c r="C32" t="s">
         <v>18</v>
       </c>
@@ -2142,7 +3068,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>15</v>
+      </c>
       <c r="C33" t="s">
         <v>20</v>
       </c>
@@ -2151,6 +3080,216 @@
       </c>
       <c r="F33" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" t="s">
+        <v>25</v>
+      </c>
+      <c r="G37" t="s">
+        <v>24</v>
+      </c>
+      <c r="I37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38">
+        <v>8</v>
+      </c>
+      <c r="F38" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39">
+        <v>255</v>
+      </c>
+      <c r="F39" t="s">
+        <v>26</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>85</v>
+      </c>
+      <c r="D42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>86</v>
+      </c>
+      <c r="D43" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="H47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Document: Update API sheet
</commit_message>
<xml_diff>
--- a/Document/ReviewDalatDesign.xlsx
+++ b/Document/ReviewDalatDesign.xlsx
@@ -15,8 +15,9 @@
     <sheet name="Giới thiệu" sheetId="1" r:id="rId1"/>
     <sheet name="Lịch sử" sheetId="2" r:id="rId2"/>
     <sheet name="Giao diện" sheetId="3" r:id="rId3"/>
-    <sheet name="API" sheetId="4" r:id="rId4"/>
-    <sheet name="Database" sheetId="5" r:id="rId5"/>
+    <sheet name="API" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="API " sheetId="6" r:id="rId5"/>
+    <sheet name="Database" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="200">
   <si>
     <t>Tên project: Review Đà lạt</t>
   </si>
@@ -880,9 +881,6 @@
     <t>reviews/place/newest</t>
   </si>
   <si>
-    <t>2. API lấy danh sách review địa điểm tốt nhất</t>
-  </si>
-  <si>
     <t>reviews/{type:place|coffee-shop|hotel|food}/{newest|best|worst}</t>
   </si>
   <si>
@@ -1004,9 +1002,6 @@
     <t>'2020-01-01 00:00:00'</t>
   </si>
   <si>
-    <t>3. API lấy comment mới nhất hiển thị ra trang chủ</t>
-  </si>
-  <si>
     <t>/comments/newest</t>
   </si>
   <si>
@@ -1690,13 +1685,1950 @@
   </si>
   <si>
     <t>review_comment</t>
+  </si>
+  <si>
+    <t>/comments/{reviewObjectId}</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"error_code"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"success"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"message"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"All got done"</t>
+    </r>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"author"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Hai Dang"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"point"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"4"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"context"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Hay lam"</t>
+    </r>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"author"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Đăng xoài"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"context"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"chuẩn mà"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"type"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"report"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"success"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"true"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"message"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"React comment success"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"data"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"[]"</t>
+    </r>
+  </si>
+  <si>
+    <t>3. API lấy danh sách review địa điểm tốt nhất</t>
+  </si>
+  <si>
+    <t>4. API lấy comment mới nhất hiển thị ra trang chủ</t>
+  </si>
+  <si>
+    <t>5. API thêm comment review object</t>
+  </si>
+  <si>
+    <t>6. API react comment review object</t>
+  </si>
+  <si>
+    <t>7. API lấy chi tiết comment</t>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"00000024"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"author"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Hai Dang"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"review_object_id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"00000001"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"context"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Hay lam"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"last_time"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"0 days 4 hours"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"comments"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: []</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"context"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Cái này hay lắm á\r\nVừa đẹp vừa xịn"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"last_time"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"387 days 14 hours"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"comments"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: [</t>
+    </r>
+  </si>
+  <si>
+    <t>            {</t>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"00000029"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"author"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Đăng xoài"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"last_time"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"0 days 0 hours"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"context"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"chuẩn mà"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"react"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"report"</t>
+    </r>
+  </si>
+  <si>
+    <t>            },</t>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"00000028"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"react"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"like"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"00000027"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"react"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>null</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"00000026"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <t>            }</t>
+  </si>
+  <si>
+    <t>        ]</t>
+  </si>
+  <si>
+    <t>8. API search review</t>
+  </si>
+  <si>
+    <t>/reviews/search?query=?</t>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"00000003"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"name"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Ga"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"image_icon"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"type"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"2"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"00000007"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"name"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Dream Comes True"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"type"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"4"</t>
+    </r>
+  </si>
+  <si>
+    <t>9. API get news detail</t>
+  </si>
+  <si>
+    <t>/news/detail/{id}</t>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"00000001"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"title"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Hello các bạn"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"title_image"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"https://www.w3schools.com/howto/img_nature_wide.jpg"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"html_content"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"&lt;p&gt;Hello babe&lt;/p&gt;"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"source"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Admin"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"created"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"2021-01-08 09:57:11"</t>
+    </r>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>Request</t>
+  </si>
+  <si>
+    <t>Logic</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>API lấy danh sách tin tức mới nhất</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  
+    {  
+        "id":"123",  
+        "title": "123",  
+        "title_image": "123",  
+        "created": "20-2-2020"  
+    },  
+    {  
+        "id":"123",  
+        "title": "123",  
+        "title_image": "123",  
+        "created": "20-2-2020"  
+    }  
+]  </t>
+  </si>
+  <si>
+    <t>API lấy danh sách review địa điểm mới nhất</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[
+    {
+        "id": "00000002",
+        "name": "Thiền viện Trúc lâm",
+        "type": "1",
+        "image_icon": "https://mdbootstrap.com/img/Photos/Avatars/img%20(31).jpg",
+        "average_rating": "3.5",
+        "all_rates": "62",
+        "location": "Hoa Cẩm Tú Cầu, Phường 3, Thành phố Đà Lạt, Lâm Đồng, Vietnam",
+        "description": "Traditional Zen Buddhist temple located on a hill &amp; featuring picturesque gardens &amp; mountain views."
+    },
+    {
+        "id": "00000001",
+        "name": "Quảng Trường",
+        "type": "1",
+        "image_icon": "https://mdbootstrap.com/img/Photos/Avatars/img%20(31).jpg",
+        "average_rating": "3.5",
+        "all_rates": "34",
+        "location": " Bà Huyện Thanh Quan, Phường 1, Thành phố Đà Lạt, Lâm Đồng\r\n",
+        "description": "Quảng trường Lâm Viên là quảng trường nằm ở đường Trần Quốc Toản, đối diện hồ Xuân Hương, Phường 10, trung tâm thành phố Đà Lạt, tỉnh Lâm Đồng."
+    }
+]
+</t>
+  </si>
+  <si>
+    <t>API lấy danh sách review địa điểm tốt nhất</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[
+    {
+        "id": "00000001",
+        "name": "Quảng Trường",
+        "type": "1",
+        "image_icon": "https://mdbootstrap.com/img/Photos/Avatars/img%20(31).jpg",
+        "average_rating": "3.5",
+        "all_rates": "34",
+        "location": " Bà Huyện Thanh Quan, Phường 1, Thành phố Đà Lạt, Lâm Đồng\r\n",
+        "description": "Quảng trường Lâm Viên là quảng trường nằm ở đường Trần Quốc Toản, đối diện hồ Xuân Hương, Phường 10, trung tâm thành phố Đà Lạt, tỉnh Lâm Đồng."
+    },
+    {
+        "id": "00000002",
+        "name": "Thiền viện Trúc lâm",
+        "type": "1",
+        "image_icon": "https://mdbootstrap.com/img/Photos/Avatars/img%20(31).jpg",
+        "average_rating": "5.0",
+        "all_rates": "22",
+        "location": "Hoa Cẩm Tú Cầu, Phường 3, Thành phố Đà Lạt, Lâm Đồng, Vietnam",
+        "description": "Traditional Zen Buddhist temple located on a hill &amp; featuring picturesque gardens &amp; mountain views."
+    }
+]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> API lấy comment mới nhất hiển thị ra trang chủ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[
+    {
+        "author": "Ông Lão Đánh Cá",
+        "review_object_id": "2",
+        "review_object_name": "Thiền viện Trúc lâm",
+        "last_time": "6 days 16 hours",
+        "point": "4",
+        "context": "Tuyệt vời ông mặt trời\t"
+    },
+    {
+        "author": "Cá Vàng",
+        "review_object_id": "4",
+        "review_object_name": "Nhà Thờ",
+        "last_time": "11 days 16 hours",
+        "point": "5",
+        "context": "Tuyệt vời ông mặt trời\t"
+    },
+    {
+        "author": "Người Bí Ẩn",
+        "review_object_id": "1",
+        "review_object_name": "Quảng Trường",
+        "last_time": "379 days 16 hours",
+        "point": "3",
+        "context": "Cái này hay lắm á\r\nVừa đẹp vừa xịn"
+    }
+]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> API thêm comment review object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+    "author":"Hai Dang",
+    "point":"4",
+    "context":"Hay lam"
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+    "success": "success",
+    "message": "All got done",
+    "data":[]
+}
+</t>
+  </si>
+  <si>
+    <t>API react comment review object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+    "author":"Đăng xoài",
+    "context":"chuẩn mà",
+    "type":"report"
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+    "success": "true",
+    "message": "React comment success",
+    "data": "[]"
+}
+</t>
+  </si>
+  <si>
+    <t>API lấy chi tiết comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[
+    {
+        "id": "00000024",
+        "author": "Hai Dang",
+        "review_object_id": "00000001",
+        "point": "4",
+        "context": "Hay lam",
+        "last_time": "0 days 4 hours",
+        "comments": []
+    },
+    {
+        "id": "00000001",
+        "author": "Người Bí Ẩn",
+        "review_object_id": "00000001",
+        "point": "3",
+        "context": "Cái này hay lắm á\r\nVừa đẹp vừa xịn",
+        "last_time": "387 days 14 hours",
+        "comments": [
+            {
+                "id": "00000029",
+                "author": "Đăng xoài",
+                "last_time": "0 days 0 hours",
+                "context": "chuẩn mà",
+                "react": "report"
+            },
+            {
+                "id": "00000028",
+                "author": "Đăng xoài",
+                "last_time": "0 days 0 hours",
+                "context": "chuẩn mà",
+                "react": "like"
+            }
+        ]
+    }
+]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[
+    {
+        "id": "00000003",
+        "name": "Ga",
+        "image_icon": null,
+        "type": "2"
+    },
+    {
+        "id": "00000007",
+        "name": "Dream Comes True",
+        "image_icon": null,
+        "type": "4"
+    }
+]
+</t>
+  </si>
+  <si>
+    <t>API get news detail</t>
+  </si>
+  <si>
+    <t>API search review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+    "id": "00000001",
+    "title": "Hello các bạn",
+    "title_image": "https://www.w3schools.com/howto/img_nature_wide.jpg",
+    "html_content": "&lt;p&gt;Hello babe&lt;/p&gt;",
+    "source": "Admin",
+    "created": "2021-01-08 09:57:11"
+}
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1717,6 +3649,13 @@
       <family val="3"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF0451A5"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <color rgb="FF0451A5"/>
       <name val="Consolas"/>
@@ -1743,12 +3682,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2093,10 +4047,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C108"/>
+  <dimension ref="B2:C227"/>
   <sheetViews>
-    <sheetView topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="J85" sqref="J85"/>
+    <sheetView topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="C220" sqref="C220:C227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2344,7 +4298,7 @@
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>77</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
@@ -2352,7 +4306,7 @@
         <v>75</v>
       </c>
       <c r="C52" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
@@ -2453,12 +4407,12 @@
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C71" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C72" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
@@ -2483,7 +4437,7 @@
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
@@ -2491,7 +4445,7 @@
         <v>75</v>
       </c>
       <c r="C80" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
@@ -2522,32 +4476,32 @@
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C85" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C86" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C87" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C88" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C89" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C90" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
@@ -2562,82 +4516,682 @@
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C93" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C94" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C95" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C96" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C97" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C98" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C99" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C100" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C101" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C102" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C103" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C102" s="1" t="s">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C104" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C103" s="1" t="s">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C105" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C104" s="1" t="s">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C106" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C105" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C106" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C107" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C108" s="1" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>75</v>
+      </c>
+      <c r="C112" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>30</v>
+      </c>
+      <c r="C113" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>29</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C115" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C116" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C117" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C118" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C119" s="1"/>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>116</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C121" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C122" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C123" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C124" s="1"/>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
+        <v>75</v>
+      </c>
+      <c r="C127" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>30</v>
+      </c>
+      <c r="C128" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>29</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C130" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C131" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C132" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C133" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>32</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C135" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C136" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C137" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C138" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C139" s="1"/>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>75</v>
+      </c>
+      <c r="C142" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>30</v>
+      </c>
+      <c r="C143" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>32</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C146" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C147" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C148" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C149" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C150" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C151" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C152" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C153" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C154" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C155" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C156" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C157" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C158" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C159" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C160" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C161" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="162" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C162" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="163" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C163" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C164" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C165" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C166" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="167" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C167" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C168" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="169" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C169" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C170" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="171" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C171" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="172" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C172" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="173" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C173" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="174" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C174" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="175" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C175" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="176" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C176" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C177" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="178" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C178" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C179" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="180" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C180" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C181" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="182" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C182" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="183" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C183" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="184" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C184" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="185" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C185" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="186" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C186" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="187" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C187" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="188" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C188" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="189" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C189" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="190" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C190" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="191" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C191" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="192" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C192" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C193" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B195" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B197" t="s">
+        <v>75</v>
+      </c>
+      <c r="C197" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B198" t="s">
+        <v>30</v>
+      </c>
+      <c r="C198" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B199" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B200" t="s">
+        <v>32</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C201" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C202" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C203" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C204" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C205" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C206" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C207" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C208" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C209" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C210" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C211" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C212" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C213" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B215" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B217" t="s">
+        <v>75</v>
+      </c>
+      <c r="C217" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="218" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
+        <v>30</v>
+      </c>
+      <c r="C218" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B219" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="220" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B220" t="s">
+        <v>32</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="221" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C221" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="222" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C222" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="223" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C223" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="224" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C224" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="225" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C225" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="226" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C226" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="227" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C227" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2648,10 +5202,225 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I49"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="33.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" customWidth="1"/>
+    <col min="6" max="6" width="54" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" ht="236.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="250.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" ht="257.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="284.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="225" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3084,12 +5853,12 @@
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
@@ -3137,7 +5906,7 @@
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D39" t="s">
         <v>14</v>
@@ -3149,12 +5918,12 @@
         <v>26</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
@@ -3165,7 +5934,7 @@
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D41" t="s">
         <v>56</v>
@@ -3173,13 +5942,10 @@
       <c r="E41">
         <v>1</v>
       </c>
-      <c r="H41">
-        <v>3</v>
-      </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
@@ -3190,7 +5956,7 @@
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D43" t="s">
         <v>16</v>
@@ -3204,7 +5970,7 @@
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -3218,7 +5984,7 @@
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D45" t="s">
         <v>12</v>
@@ -3232,7 +5998,7 @@
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
@@ -3246,21 +6012,21 @@
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="D47" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="H47" t="s">
-        <v>91</v>
+      <c r="H47">
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="D48" t="s">
         <v>19</v>
@@ -3268,27 +6034,41 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48" t="s">
-        <v>26</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>92</v>
+      <c r="H48" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D49" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" t="s">
         <v>26</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>20</v>
+      </c>
+      <c r="D50" t="s">
+        <v>56</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+      <c r="H50">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Document: update paging APIs
</commit_message>
<xml_diff>
--- a/Document/ReviewDalatDesign.xlsx
+++ b/Document/ReviewDalatDesign.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="205">
   <si>
     <t>Tên project: Review Đà lạt</t>
   </si>
@@ -3622,6 +3622,21 @@
     "created": "2021-01-08 09:57:11"
 }
 </t>
+  </si>
+  <si>
+    <t>API lấy số trang review</t>
+  </si>
+  <si>
+    <t>/reviews/{type:place|coffee-shop|hotel|food}/all-pages</t>
+  </si>
+  <si>
+    <t>{"all_pages":1}</t>
+  </si>
+  <si>
+    <t>reviews/place/newest?page=</t>
+  </si>
+  <si>
+    <t>reviews/{type:place|coffee-shop|hotel|food}/{newest|best|worst}?page=</t>
   </si>
 </sst>
 </file>
@@ -5202,18 +5217,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="7"/>
     <col min="2" max="2" width="33.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.140625" customWidth="1"/>
     <col min="6" max="6" width="54" customWidth="1"/>
@@ -5273,7 +5288,7 @@
         <v>182</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>76</v>
+        <v>203</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>31</v>
@@ -5293,7 +5308,7 @@
         <v>184</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>77</v>
+        <v>204</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>31</v>
@@ -5408,6 +5423,23 @@
       </c>
       <c r="F10" s="4" t="s">
         <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>